<commit_message>
Minor fixes in the PU-MET-FAST-019 files.
</commit_message>
<xml_diff>
--- a/PU-MET-FAST-019/PU-MET-FAST-019.xlsx
+++ b/PU-MET-FAST-019/PU-MET-FAST-019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\GitHub\ML_neutronics\PU-MET-FAST-019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D31E9F2-FFBF-445C-AEBD-0DBC260AA7A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B4356F-A6EF-46FA-88B7-D4EBE4A874B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
   <si>
     <t>Criticality Eigenvalues</t>
   </si>
@@ -162,7 +162,10 @@
     <t>Fe (99.05% density)</t>
   </si>
   <si>
-    <t>Fe (99.9% density)</t>
+    <t>Copper Cup</t>
+  </si>
+  <si>
+    <t>Cu (99.9% density)</t>
   </si>
 </sst>
 </file>
@@ -482,6 +485,168 @@
   </cellStyleXfs>
   <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -497,179 +662,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1047,7 +1050,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1061,277 +1064,277 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
-      <c r="G1" s="4" t="s">
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="61"/>
+      <c r="G1" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="5"/>
+      <c r="H1" s="63"/>
     </row>
     <row r="2" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="65"/>
+      <c r="D2" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="G2" s="9" t="s">
+      <c r="E2" s="65"/>
+      <c r="G2" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="10"/>
+      <c r="H2" s="42"/>
     </row>
     <row r="3" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="12" t="s">
+      <c r="C3" s="67"/>
+      <c r="D3" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="G3" s="14" t="s">
+      <c r="E3" s="67"/>
+      <c r="G3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="4">
         <v>15.4757</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="17" t="s">
+      <c r="C4" s="53"/>
+      <c r="D4" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="18"/>
-      <c r="G4" s="19" t="s">
+      <c r="E4" s="53"/>
+      <c r="G4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="20" t="s">
+      <c r="H4" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="14.7" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="62" t="s">
+      <c r="G5" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="66">
+      <c r="H5" s="35">
         <v>3.3930000000000002E-2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="26">
+      <c r="B6" s="12">
         <v>0.99587899999999996</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="13">
         <v>2.2399999999999998E-3</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="55">
         <v>1.0012000000000001</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="57">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="G6" s="62" t="s">
+      <c r="G6" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="66">
+      <c r="H6" s="35">
         <v>3.5043000000000001E-3</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A7" s="25"/>
-      <c r="B7" s="30">
+      <c r="A7" s="54"/>
+      <c r="B7" s="14">
         <v>0.99398399999999998</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="15">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="29"/>
-      <c r="G7" s="62" t="s">
+      <c r="D7" s="55"/>
+      <c r="E7" s="57"/>
+      <c r="G7" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="66">
+      <c r="H7" s="35">
         <v>3.9188999999999999E-4</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A8" s="25"/>
-      <c r="B8" s="30">
+      <c r="A8" s="54"/>
+      <c r="B8" s="14">
         <v>2.1365300000000002E-3</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8" s="15">
         <v>5.3150000000000003E-2</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="29"/>
-      <c r="G8" s="62" t="s">
+      <c r="D8" s="55"/>
+      <c r="E8" s="57"/>
+      <c r="G8" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="66">
+      <c r="H8" s="35">
         <v>2.2104999999999998E-3</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="30">
+      <c r="B9" s="14">
         <v>0.99983599999999995</v>
       </c>
-      <c r="C9" s="31">
+      <c r="C9" s="15">
         <v>1.3799999999999999E-3</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="29"/>
-      <c r="G9" s="62" t="s">
+      <c r="D9" s="55"/>
+      <c r="E9" s="57"/>
+      <c r="G9" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="66">
+      <c r="H9" s="35">
         <v>3.0246E-4</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="30">
+      <c r="B10" s="14">
         <v>1.0026900000000001</v>
       </c>
-      <c r="C10" s="31">
+      <c r="C10" s="15">
         <v>1.5299999999999999E-3</v>
       </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="29"/>
-      <c r="G10" s="62" t="s">
+      <c r="D10" s="55"/>
+      <c r="E10" s="57"/>
+      <c r="G10" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="H10" s="66">
+      <c r="H10" s="35">
         <v>3.2525000000000002E-4</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="30">
+      <c r="B11" s="14">
         <v>0.99983599999999995</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="15">
         <v>1.3799999999999999E-3</v>
       </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="35"/>
-      <c r="G11" s="63" t="s">
+      <c r="D11" s="56"/>
+      <c r="E11" s="58"/>
+      <c r="G11" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="66">
+      <c r="H11" s="35">
         <v>7.4099999999999999E-5</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="39">
+      <c r="B12" s="21">
         <v>3.1591300000000002</v>
       </c>
-      <c r="C12" s="40">
+      <c r="C12" s="22">
         <v>7.6000000000000004E-4</v>
       </c>
-      <c r="G12" s="64" t="s">
+      <c r="G12" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="67">
+      <c r="H12" s="36">
         <v>1.4187E-3</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="39">
+      <c r="B13" s="21">
         <v>1</v>
       </c>
-      <c r="C13" s="42">
+      <c r="C13" s="23">
         <v>0</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="10"/>
+      <c r="H13" s="42"/>
     </row>
     <row r="14" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="41"/>
-      <c r="B14" s="39">
+      <c r="A14" s="45"/>
+      <c r="B14" s="21">
         <v>1</v>
       </c>
-      <c r="C14" s="42">
+      <c r="C14" s="23">
         <v>0</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="65">
+      <c r="H14" s="34">
         <v>1.8169</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="43"/>
-      <c r="B15" s="44">
+      <c r="A15" s="46"/>
+      <c r="B15" s="24">
         <v>1</v>
       </c>
-      <c r="C15" s="45">
+      <c r="C15" s="25">
         <v>0</v>
       </c>
-      <c r="G15" s="36" t="s">
+      <c r="G15" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="37" t="s">
+      <c r="H15" s="19" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="G16" s="23" t="s">
+      <c r="G16" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="H16" s="24">
+      <c r="H16" s="11">
         <v>0.12081</v>
       </c>
     </row>
@@ -1343,15 +1346,15 @@
       <c r="C17" s="48"/>
       <c r="D17" s="48"/>
       <c r="E17" s="49"/>
-      <c r="G17" s="23" t="s">
+      <c r="G17" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="H17" s="24">
+      <c r="H17" s="11">
         <v>8.2064000000000006E-5</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="14.7" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B18" s="50" t="s">
@@ -1362,152 +1365,171 @@
         <v>4</v>
       </c>
       <c r="E18" s="51"/>
-      <c r="G18" s="23" t="s">
+      <c r="G18" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H18" s="24">
+      <c r="H18" s="11">
         <v>1.002E-4</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="52" t="s">
+      <c r="A19" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="17" t="s">
+      <c r="C19" s="53"/>
+      <c r="D19" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="18"/>
-      <c r="G19" s="46" t="s">
+      <c r="E19" s="53"/>
+      <c r="G19" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="H19" s="32">
+      <c r="H19" s="16">
         <v>5.0939000000000001E-5</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="53" t="s">
+      <c r="A20" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="54" t="s">
+      <c r="B20" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="55"/>
-      <c r="D20" s="54" t="s">
+      <c r="C20" s="44"/>
+      <c r="D20" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="55"/>
-      <c r="G20" s="9" t="s">
+      <c r="E20" s="44"/>
+      <c r="G20" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="H20" s="10"/>
+      <c r="H20" s="42"/>
     </row>
     <row r="21" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="56" t="s">
+      <c r="A21" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="57">
+      <c r="B21" s="37">
         <v>5000</v>
       </c>
-      <c r="C21" s="58"/>
-      <c r="D21" s="57">
+      <c r="C21" s="38"/>
+      <c r="D21" s="37">
         <v>1000</v>
       </c>
-      <c r="E21" s="58"/>
-      <c r="G21" s="14" t="s">
+      <c r="E21" s="38"/>
+      <c r="G21" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H21" s="65">
+      <c r="H21" s="34">
         <v>7.5278</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="14.7" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="56" t="s">
+      <c r="A22" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="57">
+      <c r="B22" s="37">
         <v>100</v>
       </c>
-      <c r="C22" s="58"/>
-      <c r="D22" s="57">
+      <c r="C22" s="38"/>
+      <c r="D22" s="37">
         <v>1010</v>
       </c>
-      <c r="E22" s="58"/>
-      <c r="G22" s="36" t="s">
+      <c r="E22" s="38"/>
+      <c r="G22" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H22" s="37" t="s">
+      <c r="H22" s="19" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="56" t="s">
+      <c r="A23" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="57">
+      <c r="B23" s="37">
         <v>20</v>
       </c>
-      <c r="C23" s="58"/>
-      <c r="D23" s="57">
+      <c r="C23" s="38"/>
+      <c r="D23" s="37">
         <v>10</v>
       </c>
-      <c r="E23" s="58"/>
-      <c r="G23" s="23" t="s">
+      <c r="E23" s="38"/>
+      <c r="G23" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="H23" s="24">
+      <c r="H23" s="11">
         <v>8.1173999999999996E-2</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="59" t="s">
+      <c r="A24" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="60">
+      <c r="B24" s="39">
         <f>B21*(B22-B23)</f>
         <v>400000</v>
       </c>
-      <c r="C24" s="61"/>
-      <c r="D24" s="60">
+      <c r="C24" s="40"/>
+      <c r="D24" s="39">
         <f>D21*(D22-D23)</f>
         <v>1000000</v>
       </c>
-      <c r="E24" s="61"/>
-      <c r="G24" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H24" s="10"/>
+      <c r="E24" s="40"/>
+      <c r="G24" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="H24" s="42"/>
     </row>
     <row r="25" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="G25" s="14" t="s">
+      <c r="G25" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H25" s="65">
+      <c r="H25" s="34">
         <v>8.6913</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="14.7" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="G26" s="36" t="s">
+      <c r="G26" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H26" s="37" t="s">
+      <c r="H26" s="19" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="G27" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="H27" s="32">
+      <c r="G27" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="H27" s="16">
         <v>8.2364999999999994E-2</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="14.7" thickTop="1" x14ac:dyDescent="0.5"/>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="D6:D11"/>
+    <mergeCell ref="E6:E11"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="B24:C24"/>
@@ -1520,25 +1542,6 @@
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="D22:E22"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="D6:D11"/>
-    <mergeCell ref="E6:E11"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>